<commit_message>
More new quest/gossip rows and some quest text changed based on gameplay testing
</commit_message>
<xml_diff>
--- a/corrections/corrections.xlsx
+++ b/corrections/corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\wow_vo_deps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\wow_vo_webui\corrections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD3ED0A-8168-4651-80BF-AB968F24B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D43FA5F-F777-49F7-A63B-429F6E1D92E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quest" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="129">
   <si>
     <t>source</t>
   </si>
@@ -441,6 +441,28 @@
   <si>
     <t>Eager for work, I see. Lucky for you a day never goes by that I don't wish I had a fledgling adventurer to perform my bidding. You see,  I can make you very happy and provide you with things you never dreamed of having, But in order for that to happen you must bring me certain items. My business in the forest often requires certain, reagents. Fetch for me 3 Nightsaber Fangs, 3 Strigid Owl Feathers and 3 swatches of Webwood Spider Silk. Let's keep this our little secret.</t>
   </si>
+  <si>
+    <t>The following items have been stolen:
+One Dark Iron Tuyere, One Lookout's Spyglass.
+A reward is being offered to individuals who find and return these pilfered items.
+The Thorium Brotherhood is certain that these items were stolen by unscrupulous and jealous Dark Iron dwarves that inhabit the Searing Gorge.
+The spyglass in question was an excellent tool for the lookouts and the tuyere was an irreplaceable smithing tool.
+Should you find the missing items, return them to Scrange.</t>
+  </si>
+  <si>
+    <t>gossip</t>
+  </si>
+  <si>
+    <t>My purpose is to regulate access to the Uldum complex for the Creators. I allow entry into the compound only when the solicitor exhibits for access the proper sequencing discs.
+Your disc set currently does not contain the Plates of Uldum, the primary prerequisite for entry. Access is not granted unless the Plates of Uldum are present.</t>
+  </si>
+  <si>
+    <t>Wanted: A skilled fighter to deal with the threat of the terror-dax that inhabit the oohn-Goro Crater. Their numbers are growing, and they are becoming a menace to travelers in the area.
+Decrease the population by slaying 10 frenzied terror-dax; Speak with Spraggle Frock after completing the task for a reward.</t>
+  </si>
+  <si>
+    <t>The flight is aware of your work in the Searing Gorge. Show it to me. The molt; imbecile!</t>
+  </si>
 </sst>
 </file>
 
@@ -828,11 +850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56545B79-22C0-4057-A076-1E697524330B}">
-  <dimension ref="A1:F1119"/>
+  <dimension ref="A1:F1123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1120" sqref="E1120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1124" sqref="D1124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9782,6 +9804,47 @@
       </c>
       <c r="E1119">
         <v>1</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1120" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1120">
+        <v>7728</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1121" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1122" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1122">
+        <v>4501</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1123" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1123">
+        <v>4022</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -9800,11 +9863,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D60A7C4-82C4-4AAF-A00A-127D625F91A3}">
-  <dimension ref="A1:H641"/>
+  <dimension ref="A1:H691"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A616" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D643" sqref="D643"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A675" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E690" sqref="E690"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13461,7 +13524,7 @@
         <v>7918</v>
       </c>
       <c r="E428" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -14366,7 +14429,7 @@
         <v>7172</v>
       </c>
       <c r="E540" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
@@ -15180,6 +15243,406 @@
         <v>16458</v>
       </c>
       <c r="B641">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642">
+        <v>15549</v>
+      </c>
+      <c r="B642">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A643">
+        <v>15556</v>
+      </c>
+      <c r="B643">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A644">
+        <v>15557</v>
+      </c>
+      <c r="B644">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A645">
+        <v>15558</v>
+      </c>
+      <c r="B645">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A646">
+        <v>15559</v>
+      </c>
+      <c r="B646">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647">
+        <v>15560</v>
+      </c>
+      <c r="B647">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648">
+        <v>15561</v>
+      </c>
+      <c r="B648">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649">
+        <v>15562</v>
+      </c>
+      <c r="B649">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A650">
+        <v>15563</v>
+      </c>
+      <c r="B650">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651">
+        <v>15564</v>
+      </c>
+      <c r="B651">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A652">
+        <v>15565</v>
+      </c>
+      <c r="B652">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653">
+        <v>15566</v>
+      </c>
+      <c r="B653">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654">
+        <v>15567</v>
+      </c>
+      <c r="B654">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655">
+        <v>15568</v>
+      </c>
+      <c r="B655">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656">
+        <v>15569</v>
+      </c>
+      <c r="B656">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657">
+        <v>15570</v>
+      </c>
+      <c r="B657">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A658">
+        <v>15572</v>
+      </c>
+      <c r="B658">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A659">
+        <v>15573</v>
+      </c>
+      <c r="B659">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A660">
+        <v>15574</v>
+      </c>
+      <c r="B660">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A661">
+        <v>15575</v>
+      </c>
+      <c r="B661">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A662">
+        <v>15576</v>
+      </c>
+      <c r="B662">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A663">
+        <v>15577</v>
+      </c>
+      <c r="B663">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664">
+        <v>15578</v>
+      </c>
+      <c r="B664">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A665">
+        <v>15579</v>
+      </c>
+      <c r="B665">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A666">
+        <v>15581</v>
+      </c>
+      <c r="B666">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A667">
+        <v>15582</v>
+      </c>
+      <c r="B667">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A668">
+        <v>15583</v>
+      </c>
+      <c r="B668">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A669">
+        <v>15584</v>
+      </c>
+      <c r="B669">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670">
+        <v>15585</v>
+      </c>
+      <c r="B670">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A671">
+        <v>15586</v>
+      </c>
+      <c r="B671">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A672">
+        <v>15587</v>
+      </c>
+      <c r="B672">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A673">
+        <v>15588</v>
+      </c>
+      <c r="B673">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A674">
+        <v>15592</v>
+      </c>
+      <c r="B674">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A675">
+        <v>15593</v>
+      </c>
+      <c r="B675">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A676">
+        <v>15594</v>
+      </c>
+      <c r="B676">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677">
+        <v>15595</v>
+      </c>
+      <c r="B677">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678">
+        <v>15596</v>
+      </c>
+      <c r="B678">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679">
+        <v>15597</v>
+      </c>
+      <c r="B679">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680">
+        <v>15598</v>
+      </c>
+      <c r="B680">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681">
+        <v>15599</v>
+      </c>
+      <c r="B681">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682">
+        <v>15600</v>
+      </c>
+      <c r="B682">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683">
+        <v>15601</v>
+      </c>
+      <c r="B683">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684">
+        <v>15602</v>
+      </c>
+      <c r="B684">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685">
+        <v>15603</v>
+      </c>
+      <c r="B685">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686">
+        <v>15604</v>
+      </c>
+      <c r="B686">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687">
+        <v>15605</v>
+      </c>
+      <c r="B687">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688">
+        <v>15606</v>
+      </c>
+      <c r="B688">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689">
+        <v>15607</v>
+      </c>
+      <c r="B689">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690">
+        <v>15871</v>
+      </c>
+      <c r="B690">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691">
+        <v>15580</v>
+      </c>
+      <c r="B691">
         <v>0</v>
       </c>
     </row>
@@ -15188,10 +15651,10 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A501 A503:A641">
+  <conditionalFormatting sqref="A2:A501 A503:A650">
     <cfRule type="duplicateValues" dxfId="1" priority="92"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A641">
+  <conditionalFormatting sqref="A2:A650">
     <cfRule type="duplicateValues" dxfId="0" priority="95"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>